<commit_message>
Updated Excel peaks file.
</commit_message>
<xml_diff>
--- a/Figures/Peaks_from_Cluster_FSL_and_AFNI.xlsx
+++ b/Figures/Peaks_from_Cluster_FSL_and_AFNI.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="19440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="For_presentation_Farah" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
   <si>
     <t>Value</t>
   </si>
@@ -90,48 +91,12 @@
     <t>Region from AAL (closer b/c used single_sub_t1 brain, which this was based on)?</t>
   </si>
   <si>
-    <t>R medial frontal gyrus</t>
-  </si>
-  <si>
     <t>Hemisphere</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>R Cingulum_Ant</t>
-  </si>
-  <si>
-    <t>Paracentral_Lobule_R</t>
-  </si>
-  <si>
-    <t>Frontal_Sup_Medial_L</t>
-  </si>
-  <si>
-    <t>Cingulum_Mid_R</t>
-  </si>
-  <si>
-    <t>Supp_Motor_Area_L</t>
-  </si>
-  <si>
-    <t>Supp_Motor_Area_R</t>
-  </si>
-  <si>
-    <t>Precentral_R</t>
-  </si>
-  <si>
-    <t>Cingulum_Mid_L</t>
-  </si>
-  <si>
-    <t>Precuneus_L</t>
-  </si>
-  <si>
-    <t>Rectus_L</t>
-  </si>
-  <si>
-    <t>Frontal_Sup_R</t>
-  </si>
-  <si>
     <t>Frontal Pole</t>
   </si>
   <si>
@@ -181,6 +146,45 @@
   </si>
   <si>
     <t>Limbic</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Supplementary motor area</t>
+  </si>
+  <si>
+    <t>Medial frontal gyrus</t>
+  </si>
+  <si>
+    <t>Anterior cingulate gyrus</t>
+  </si>
+  <si>
+    <t>Paracentral lobule</t>
+  </si>
+  <si>
+    <t>Midcingulate area</t>
+  </si>
+  <si>
+    <t>Precentral gyrus</t>
+  </si>
+  <si>
+    <t>Precuneus</t>
+  </si>
+  <si>
+    <t>Gyrus rectus</t>
+  </si>
+  <si>
+    <t>Superior frontal gyrus</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Cluster</t>
   </si>
 </sst>
 </file>
@@ -241,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -249,8 +253,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -280,15 +308,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -303,6 +382,23 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -317,6 +413,23 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,7 +762,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -665,45 +778,48 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="16" thickTop="1">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>3.88</v>
       </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
       <c r="D3">
         <v>10</v>
       </c>
@@ -717,13 +833,13 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -734,7 +850,7 @@
         <v>3.88</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -749,13 +865,13 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -765,6 +881,9 @@
       <c r="B5">
         <v>3.4</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
       <c r="D5">
         <v>6</v>
       </c>
@@ -778,13 +897,13 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -794,6 +913,9 @@
       <c r="B6">
         <v>3.33</v>
       </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
       <c r="D6">
         <v>2</v>
       </c>
@@ -804,16 +926,16 @@
         <v>56</v>
       </c>
       <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
         <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -823,6 +945,9 @@
       <c r="B7">
         <v>3.22</v>
       </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
       <c r="D7">
         <v>2</v>
       </c>
@@ -836,13 +961,13 @@
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -852,6 +977,9 @@
       <c r="B8">
         <v>3.1</v>
       </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
       <c r="D8">
         <v>-10</v>
       </c>
@@ -865,13 +993,13 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -881,6 +1009,9 @@
       <c r="B9">
         <v>2.85</v>
       </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
       <c r="D9">
         <v>2</v>
       </c>
@@ -894,13 +1025,13 @@
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -910,6 +1041,9 @@
       <c r="B10">
         <v>2.57</v>
       </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
       <c r="D10">
         <v>2</v>
       </c>
@@ -920,16 +1054,16 @@
         <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -939,6 +1073,9 @@
       <c r="B11">
         <v>2.46</v>
       </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
       <c r="D11">
         <v>18</v>
       </c>
@@ -952,13 +1089,13 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -968,6 +1105,9 @@
       <c r="B12">
         <v>2.44</v>
       </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
       <c r="D12">
         <v>-10</v>
       </c>
@@ -981,13 +1121,13 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -997,7 +1137,9 @@
       <c r="B13" s="2">
         <v>2.39</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D13" s="2">
         <v>-14</v>
       </c>
@@ -1008,16 +1150,16 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
         <v>50</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" t="s">
-        <v>34</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>18</v>
@@ -1030,6 +1172,9 @@
       <c r="B14">
         <v>2.02</v>
       </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
       <c r="D14">
         <v>-10</v>
       </c>
@@ -1043,16 +1188,16 @@
         <v>11</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I14" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1062,6 +1207,9 @@
       <c r="B15">
         <v>1.89</v>
       </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
       <c r="D15">
         <v>14</v>
       </c>
@@ -1075,13 +1223,13 @@
         <v>32</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1091,6 +1239,9 @@
       <c r="B16">
         <v>1.61</v>
       </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
       <c r="D16">
         <v>18</v>
       </c>
@@ -1104,13 +1255,13 @@
         <v>9</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1118,30 +1269,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="16" thickBot="1">
+      <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="16" thickTop="1">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1461,6 +1612,468 @@
       </c>
       <c r="I33">
         <v>20.396000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" thickTop="1">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>3.88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10">
+        <v>48</v>
+      </c>
+      <c r="H3" s="10">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="10">
+        <v>3.88</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="10">
+        <v>14</v>
+      </c>
+      <c r="F4" s="10">
+        <v>58</v>
+      </c>
+      <c r="G4" s="10">
+        <v>12</v>
+      </c>
+      <c r="H4" s="10">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10">
+        <v>46</v>
+      </c>
+      <c r="G5" s="10">
+        <v>-8</v>
+      </c>
+      <c r="H5" s="10">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3.33</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>-30</v>
+      </c>
+      <c r="G6" s="10">
+        <v>56</v>
+      </c>
+      <c r="H6" s="10">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3.22</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>46</v>
+      </c>
+      <c r="G7" s="10">
+        <v>24</v>
+      </c>
+      <c r="H7" s="10">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="10">
+        <v>-10</v>
+      </c>
+      <c r="F8" s="10">
+        <v>-2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>52</v>
+      </c>
+      <c r="H8" s="10">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.85</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-26</v>
+      </c>
+      <c r="G9" s="10">
+        <v>32</v>
+      </c>
+      <c r="H9" s="10">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2.57</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>-10</v>
+      </c>
+      <c r="G10" s="10">
+        <v>68</v>
+      </c>
+      <c r="H10" s="10">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2.46</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="10">
+        <v>18</v>
+      </c>
+      <c r="F11" s="10">
+        <v>-14</v>
+      </c>
+      <c r="G11" s="10">
+        <v>80</v>
+      </c>
+      <c r="H11" s="10">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2.44</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="10">
+        <v>-10</v>
+      </c>
+      <c r="F12" s="10">
+        <v>18</v>
+      </c>
+      <c r="G12" s="10">
+        <v>40</v>
+      </c>
+      <c r="H12" s="10">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2.39</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="11">
+        <v>-14</v>
+      </c>
+      <c r="F13" s="11">
+        <v>-46</v>
+      </c>
+      <c r="G13" s="11">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2.02</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10">
+        <v>-10</v>
+      </c>
+      <c r="F14" s="10">
+        <v>26</v>
+      </c>
+      <c r="G14" s="10">
+        <v>-16</v>
+      </c>
+      <c r="H14" s="10">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.89</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="10">
+        <v>14</v>
+      </c>
+      <c r="F15" s="10">
+        <v>26</v>
+      </c>
+      <c r="G15" s="10">
+        <v>32</v>
+      </c>
+      <c r="H15" s="10">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1.61</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="10">
+        <v>18</v>
+      </c>
+      <c r="F16" s="10">
+        <v>58</v>
+      </c>
+      <c r="G16" s="10">
+        <v>32</v>
+      </c>
+      <c r="H16" s="10">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculated percentage of cluster from Yeo masks.
</commit_message>
<xml_diff>
--- a/Figures/Peaks_from_Cluster_FSL_and_AFNI.xlsx
+++ b/Figures/Peaks_from_Cluster_FSL_and_AFNI.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="19780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
   <si>
     <t>Value</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Cluster</t>
+  </si>
+  <si>
+    <t>BA (from Yale BioImage Suite package)</t>
+  </si>
+  <si>
+    <t>N/A (but 32 from Joe?)</t>
   </si>
 </sst>
 </file>
@@ -759,26 +765,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="7" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="34.1640625" customWidth="1"/>
-    <col min="10" max="10" width="65" customWidth="1"/>
+    <col min="8" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="34.1640625" customWidth="1"/>
+    <col min="11" max="11" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="16" thickBot="1">
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -798,19 +804,22 @@
         <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" thickTop="1">
+    <row r="3" spans="1:12" ht="16" thickTop="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -832,17 +841,20 @@
       <c r="G3">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>2</v>
       </c>
@@ -864,17 +876,20 @@
       <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>3</v>
       </c>
@@ -896,17 +911,20 @@
       <c r="G5">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>4</v>
       </c>
@@ -925,20 +943,23 @@
       <c r="F6">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>5</v>
       </c>
@@ -958,19 +979,22 @@
         <v>24</v>
       </c>
       <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>6</v>
       </c>
@@ -992,17 +1016,20 @@
       <c r="G8">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1024,17 +1051,20 @@
       <c r="G9">
         <v>23</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1053,20 +1083,23 @@
       <c r="F10">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>40</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>29</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1088,17 +1121,20 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
         <v>40</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1118,19 +1154,22 @@
         <v>40</v>
       </c>
       <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
         <v>32</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>38</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1149,23 +1188,26 @@
       <c r="F13" s="2">
         <v>48</v>
       </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="2">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>31</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1187,20 +1229,23 @@
       <c r="G14">
         <v>11</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1220,19 +1265,22 @@
         <v>32</v>
       </c>
       <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15">
         <v>32</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>26</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1254,22 +1302,25 @@
       <c r="G16">
         <v>9</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>25</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="16" thickBot="1">
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="16" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -1285,14 +1336,14 @@
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" thickTop="1">
+    <row r="20" spans="1:10" ht="16" thickTop="1">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1308,14 +1359,14 @@
       <c r="F20" t="s">
         <v>14</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>12</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1331,14 +1382,14 @@
       <c r="F21">
         <v>48</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>3</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1354,14 +1405,14 @@
       <c r="F22">
         <v>12</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>20.396000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1377,14 +1428,14 @@
       <c r="F23">
         <v>-8</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>3</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>24.658000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1400,14 +1451,14 @@
       <c r="F24">
         <v>56</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>3</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>22.626999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1423,14 +1474,14 @@
       <c r="F25">
         <v>24</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>5</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>20.785</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1446,14 +1497,14 @@
       <c r="F26">
         <v>52</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>2</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>20.785</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1469,14 +1520,14 @@
       <c r="F27">
         <v>32</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>24.331</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1492,14 +1543,14 @@
       <c r="F28">
         <v>68</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>20.396000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1515,14 +1566,14 @@
       <c r="F29">
         <v>80</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>4</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>20.396000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1538,14 +1589,14 @@
       <c r="F30">
         <v>40</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>23.324000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1561,14 +1612,14 @@
       <c r="F31">
         <v>-16</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>26.832999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1584,14 +1635,14 @@
       <c r="F32">
         <v>56</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>22.626999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>13</v>
       </c>
@@ -1607,10 +1658,10 @@
       <c r="F33">
         <v>32</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>20.396000000000001</v>
       </c>
     </row>

</xml_diff>